<commit_message>
fixing the indeces and columns
</commit_message>
<xml_diff>
--- a/Impact/impact_1.xlsx
+++ b/Impact/impact_1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>Investment</t>
   </si>
@@ -100,7 +100,10 @@
     <t>kha</t>
   </si>
   <si>
-    <t>single</t>
+    <t>Shading Trees</t>
+  </si>
+  <si>
+    <t>baseline</t>
   </si>
 </sst>
 </file>
@@ -458,107 +461,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:23">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:24">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
-        <v>22</v>
-      </c>
+    <row r="2" spans="1:24">
+      <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="J2" s="1" t="s">
         <v>22</v>
       </c>
@@ -566,17 +566,17 @@
         <v>22</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P2" s="1" t="s">
         <v>22</v>
       </c>
@@ -584,69 +584,99 @@
         <v>22</v>
       </c>
       <c r="R2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="U2" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="V2" s="1" t="s">
         <v>22</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="X2" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:24">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4">
         <v>1.000000158324838</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>0.9354393007233739</v>
       </c>
+      <c r="E4">
+        <v>0.9354391526201219</v>
+      </c>
       <c r="F4">
+        <v>1.06901661877103</v>
+      </c>
+      <c r="G4">
         <v>0.04106397050782107</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.05008577914486523</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.003466384087914776</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0.08160151727497578</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>0.07793689612299204</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>0.06345285149291158</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>0.0005181713204365224</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>0.0009185673316096654</v>
       </c>
-      <c r="N4">
-        <v>1.404879185429309e-06</v>
-      </c>
       <c r="O4">
+        <v>1.404879185429309E-06</v>
+      </c>
+      <c r="P4">
         <v>0.06491394690237939</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>0.09720575390383601</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>0.00409148377366364</v>
+      </c>
+      <c r="S4">
+        <v>-0.8207612388359848</v>
+      </c>
+      <c r="T4">
+        <v>-1.000797015565695</v>
+      </c>
+      <c r="U4">
+        <v>-0.06932627687911008</v>
+      </c>
+      <c r="V4">
+        <v>-1.567116398597136</v>
+      </c>
+      <c r="W4">
+        <v>-1.171851275954396</v>
+      </c>
+      <c r="X4">
+        <v>-1.554646438686177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>